<commit_message>
Update performance dashboard 2025-12-25 00:09 - Simplified Design v3.0
</commit_message>
<xml_diff>
--- a/performance-dashboard/archive/Trading_Performance_20251225.xlsx
+++ b/performance-dashboard/archive/Trading_Performance_20251225.xlsx
@@ -1296,26 +1296,26 @@
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>¥1,003,142.00</t>
+          <t>¥1,005,052.00</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>¥+3,142.00</t>
+          <t>¥+5,052.00</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>+0.31%</t>
+          <t>+0.51%</t>
         </is>
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>+16.98%</t>
+          <t>+23.36%</t>
         </is>
       </c>
       <c r="H12" t="n">
-        <v>14.046</v>
+        <v>17.501</v>
       </c>
       <c r="I12" t="inlineStr">
         <is>
@@ -1324,24 +1324,24 @@
       </c>
       <c r="J12" t="inlineStr">
         <is>
-          <t>50.0%</t>
+          <t>60.0%</t>
         </is>
       </c>
       <c r="K12" t="inlineStr">
         <is>
-          <t>0.0785%</t>
+          <t>0.1009%</t>
         </is>
       </c>
       <c r="L12" t="inlineStr">
         <is>
-          <t>0.0794%</t>
+          <t>0.0840%</t>
         </is>
       </c>
       <c r="M12" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="N12" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="O12" t="inlineStr">
         <is>
@@ -1350,7 +1350,7 @@
       </c>
       <c r="P12" t="inlineStr">
         <is>
-          <t>20251223</t>
+          <t>20251224</t>
         </is>
       </c>
     </row>
@@ -2739,26 +2739,26 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>¥1,003,142.00</t>
+          <t>¥1,005,052.00</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>¥+3,142.00</t>
+          <t>¥+5,052.00</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>+0.31%</t>
+          <t>+0.51%</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>+16.98%</t>
+          <t>+23.36%</t>
         </is>
       </c>
       <c r="H2" t="n">
-        <v>14.046</v>
+        <v>17.501</v>
       </c>
       <c r="I2" t="inlineStr">
         <is>
@@ -2767,24 +2767,24 @@
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>50.0%</t>
+          <t>60.0%</t>
         </is>
       </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t>0.0785%</t>
+          <t>0.1009%</t>
         </is>
       </c>
       <c r="L2" t="inlineStr">
         <is>
-          <t>0.0794%</t>
+          <t>0.0840%</t>
         </is>
       </c>
       <c r="M2" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="N2" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="O2" t="inlineStr">
         <is>
@@ -2793,7 +2793,7 @@
       </c>
       <c r="P2" t="inlineStr">
         <is>
-          <t>20251223</t>
+          <t>20251224</t>
         </is>
       </c>
     </row>

</xml_diff>